<commit_message>
end of day 17 november 2025
</commit_message>
<xml_diff>
--- a/Daily Activities.xlsx
+++ b/Daily Activities.xlsx
@@ -244,7 +244,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="303">
   <si>
     <t>DATE</t>
   </si>
@@ -789,18 +789,27 @@
     <t>Done ordering 5 bags</t>
   </si>
   <si>
-    <t>List suppliier status on galungan</t>
+    <t>Goods already arrived</t>
+  </si>
+  <si>
+    <t>Check suppliier status on galungan</t>
   </si>
   <si>
     <t>Order teh teh botol kotak 2 dos</t>
   </si>
   <si>
+    <t>Ordered</t>
+  </si>
+  <si>
     <t>Go to Pertamina to get change for petty cash</t>
   </si>
   <si>
     <t>Make paid suppliier lists</t>
   </si>
   <si>
+    <t>Done. need to filled up the data</t>
+  </si>
+  <si>
     <t>Sending service lists to Rhoma</t>
   </si>
   <si>
@@ -820,6 +829,18 @@
   </si>
   <si>
     <t>Print new balagan stickers (Ms. Angelica)</t>
+  </si>
+  <si>
+    <t>AC Cinema got leaking again</t>
+  </si>
+  <si>
+    <t>Already make report</t>
+  </si>
+  <si>
+    <t>AC Cinema is leaking again</t>
+  </si>
+  <si>
+    <t>Already make report to aircond solution</t>
   </si>
   <si>
     <t>Trip</t>
@@ -2089,7 +2110,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2507,23 +2528,14 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3064,18 +3076,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K193"/>
+  <dimension ref="A1:K215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B191" sqref="B191"/>
+      <selection pane="bottomLeft" activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.8571428571429" style="94"/>
-    <col min="2" max="2" width="87" customWidth="1"/>
+    <col min="2" max="2" width="97" customWidth="1"/>
     <col min="3" max="3" width="71.1428571428571" style="95" customWidth="1"/>
     <col min="4" max="4" width="9.14285714285714" style="96"/>
     <col min="6" max="6" width="12.8571428571429"/>
@@ -5220,11 +5232,11 @@
       <c r="B179" s="110" t="s">
         <v>161</v>
       </c>
-      <c r="C179" s="128" t="s">
-        <v>173</v>
+      <c r="C179" s="111" t="s">
+        <v>181</v>
       </c>
       <c r="D179" s="118" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -5277,126 +5289,380 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="138"/>
-      <c r="B184" s="139" t="s">
-        <v>181</v>
-      </c>
-      <c r="C184" s="140" t="s">
-        <v>101</v>
-      </c>
-      <c r="D184" s="141" t="s">
-        <v>53</v>
+      <c r="B184" s="110" t="s">
+        <v>182</v>
+      </c>
+      <c r="C184" s="111" t="s">
+        <v>175</v>
+      </c>
+      <c r="D184" s="118" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="138"/>
-      <c r="B185" s="139" t="s">
-        <v>182</v>
-      </c>
-      <c r="C185" s="140" t="s">
-        <v>101</v>
-      </c>
-      <c r="D185" s="141" t="s">
-        <v>53</v>
+      <c r="B185" s="110" t="s">
+        <v>183</v>
+      </c>
+      <c r="C185" s="111" t="s">
+        <v>184</v>
+      </c>
+      <c r="D185" s="118" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="138"/>
-      <c r="B186" s="139" t="s">
-        <v>183</v>
-      </c>
-      <c r="C186" s="140" t="s">
+      <c r="B186" s="110" t="s">
+        <v>185</v>
+      </c>
+      <c r="C186" s="128" t="s">
         <v>101</v>
       </c>
-      <c r="D186" s="141" t="s">
+      <c r="D186" s="118" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="138"/>
-      <c r="B187" s="139" t="s">
-        <v>184</v>
-      </c>
-      <c r="C187" s="140" t="s">
-        <v>101</v>
-      </c>
-      <c r="D187" s="141" t="s">
+      <c r="B187" s="110" t="s">
+        <v>186</v>
+      </c>
+      <c r="C187" s="128" t="s">
+        <v>187</v>
+      </c>
+      <c r="D187" s="118" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" s="138"/>
-      <c r="B188" s="139" t="s">
-        <v>185</v>
-      </c>
-      <c r="C188" s="142" t="s">
+      <c r="B188" s="110" t="s">
+        <v>188</v>
+      </c>
+      <c r="C188" s="111" t="s">
         <v>175</v>
       </c>
-      <c r="D188" s="141" t="s">
-        <v>53</v>
+      <c r="D188" s="118" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" s="138"/>
-      <c r="B189" s="139" t="s">
-        <v>186</v>
-      </c>
-      <c r="C189" s="143" t="s">
-        <v>187</v>
-      </c>
-      <c r="D189" s="141" t="s">
+      <c r="B189" s="110" t="s">
+        <v>189</v>
+      </c>
+      <c r="C189" s="129" t="s">
+        <v>190</v>
+      </c>
+      <c r="D189" s="118" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" s="138"/>
-      <c r="B190" s="139" t="s">
-        <v>184</v>
-      </c>
-      <c r="C190" s="142" t="s">
+      <c r="B190" s="110" t="s">
+        <v>186</v>
+      </c>
+      <c r="C190" s="111" t="s">
         <v>175</v>
       </c>
-      <c r="D190" s="141" t="s">
-        <v>53</v>
+      <c r="D190" s="118" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="138"/>
-      <c r="B191" s="139" t="s">
-        <v>188</v>
-      </c>
-      <c r="C191" s="140" t="s">
-        <v>189</v>
-      </c>
-      <c r="D191" s="141" t="s">
+      <c r="B191" s="110" t="s">
+        <v>191</v>
+      </c>
+      <c r="C191" s="128" t="s">
+        <v>192</v>
+      </c>
+      <c r="D191" s="118" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" s="138"/>
-      <c r="B192" s="139" t="s">
+      <c r="B192" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C192" s="128" t="s">
+        <v>101</v>
+      </c>
+      <c r="D192" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="138"/>
+      <c r="B193" s="110" t="s">
+        <v>194</v>
+      </c>
+      <c r="C193" s="128" t="s">
+        <v>101</v>
+      </c>
+      <c r="D193" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="139"/>
+      <c r="B194" s="140" t="s">
+        <v>195</v>
+      </c>
+      <c r="C194" s="141" t="s">
+        <v>196</v>
+      </c>
+      <c r="D194" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="137">
+        <v>45979</v>
+      </c>
+      <c r="B196" s="135" t="s">
+        <v>56</v>
+      </c>
+      <c r="C196" s="128" t="s">
+        <v>110</v>
+      </c>
+      <c r="D196" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" s="138"/>
+      <c r="B197" s="135" t="s">
+        <v>100</v>
+      </c>
+      <c r="C197" s="128" t="s">
+        <v>147</v>
+      </c>
+      <c r="D197" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="138"/>
+      <c r="B198" s="135" t="s">
+        <v>148</v>
+      </c>
+      <c r="C198" s="128" t="s">
+        <v>138</v>
+      </c>
+      <c r="D198" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" s="138"/>
+      <c r="B199" s="110" t="s">
+        <v>111</v>
+      </c>
+      <c r="C199" s="128" t="s">
+        <v>160</v>
+      </c>
+      <c r="D199" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="138"/>
+      <c r="B200" s="110" t="s">
+        <v>161</v>
+      </c>
+      <c r="C200" s="111" t="s">
+        <v>181</v>
+      </c>
+      <c r="D200" s="118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="138"/>
+      <c r="B201" s="110" t="s">
+        <v>132</v>
+      </c>
+      <c r="C201" s="128" t="s">
+        <v>155</v>
+      </c>
+      <c r="D201" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" s="138"/>
+      <c r="B202" s="110" t="s">
+        <v>164</v>
+      </c>
+      <c r="C202" s="100" t="s">
+        <v>165</v>
+      </c>
+      <c r="D202" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="138"/>
+      <c r="B203" s="110" t="s">
+        <v>169</v>
+      </c>
+      <c r="C203" s="128" t="s">
+        <v>170</v>
+      </c>
+      <c r="D203" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="138"/>
+      <c r="B204" s="110" t="s">
+        <v>176</v>
+      </c>
+      <c r="C204" s="128" t="s">
+        <v>101</v>
+      </c>
+      <c r="D204" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" s="138"/>
+      <c r="B205" s="110" t="s">
+        <v>182</v>
+      </c>
+      <c r="C205" s="111" t="s">
+        <v>175</v>
+      </c>
+      <c r="D205" s="118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" s="138"/>
+      <c r="B206" s="110" t="s">
+        <v>183</v>
+      </c>
+      <c r="C206" s="111" t="s">
+        <v>184</v>
+      </c>
+      <c r="D206" s="118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" s="138"/>
+      <c r="B207" s="110" t="s">
+        <v>185</v>
+      </c>
+      <c r="C207" s="128" t="s">
+        <v>101</v>
+      </c>
+      <c r="D207" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" s="138"/>
+      <c r="B208" s="110" t="s">
+        <v>186</v>
+      </c>
+      <c r="C208" s="128" t="s">
+        <v>187</v>
+      </c>
+      <c r="D208" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" s="138"/>
+      <c r="B209" s="110" t="s">
+        <v>188</v>
+      </c>
+      <c r="C209" s="111" t="s">
+        <v>175</v>
+      </c>
+      <c r="D209" s="118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" s="138"/>
+      <c r="B210" s="110" t="s">
+        <v>189</v>
+      </c>
+      <c r="C210" s="129" t="s">
         <v>190</v>
       </c>
-      <c r="C192" s="140" t="s">
+      <c r="D210" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" s="138"/>
+      <c r="B211" s="110" t="s">
+        <v>186</v>
+      </c>
+      <c r="C211" s="111" t="s">
+        <v>175</v>
+      </c>
+      <c r="D211" s="118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="138"/>
+      <c r="B212" s="110" t="s">
+        <v>191</v>
+      </c>
+      <c r="C212" s="128" t="s">
+        <v>192</v>
+      </c>
+      <c r="D212" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="138"/>
+      <c r="B213" s="110" t="s">
+        <v>193</v>
+      </c>
+      <c r="C213" s="128" t="s">
         <v>101</v>
       </c>
-      <c r="D192" s="141" t="s">
+      <c r="D213" s="118" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="193" spans="1:4">
-      <c r="A193" s="144"/>
-      <c r="B193" s="139" t="s">
-        <v>191</v>
-      </c>
-      <c r="C193" s="140" t="s">
+    <row r="214" spans="1:4">
+      <c r="A214" s="138"/>
+      <c r="B214" s="110" t="s">
+        <v>194</v>
+      </c>
+      <c r="C214" s="128" t="s">
         <v>101</v>
       </c>
-      <c r="D193" s="141" t="s">
+      <c r="D214" s="118" t="s">
         <v>53</v>
       </c>
     </row>
+    <row r="215" spans="1:4">
+      <c r="A215" s="139"/>
+      <c r="B215" s="140" t="s">
+        <v>197</v>
+      </c>
+      <c r="C215" s="141" t="s">
+        <v>198</v>
+      </c>
+      <c r="D215" s="118" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="A2:A15"/>
     <mergeCell ref="A17:A21"/>
@@ -5414,7 +5680,8 @@
     <mergeCell ref="A136:A146"/>
     <mergeCell ref="A148:A159"/>
     <mergeCell ref="A161:A173"/>
-    <mergeCell ref="A175:A193"/>
+    <mergeCell ref="A175:A194"/>
+    <mergeCell ref="A196:A215"/>
     <mergeCell ref="D24:D25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5461,29 +5728,29 @@
         <v>7</v>
       </c>
       <c r="B1" s="74" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="C1" s="74" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="74" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="E1" s="74" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="F1" s="74" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="G1" s="74" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="H1" s="74" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="I1" s="88"/>
       <c r="J1" s="89" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" s="68" customFormat="1" spans="1:10">
@@ -5491,10 +5758,10 @@
         <v>45954</v>
       </c>
       <c r="B2" s="76" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C2" s="77" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D2" s="78">
         <v>16</v>
@@ -5522,10 +5789,10 @@
         <v>45956</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C3" s="82" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D3" s="83">
         <v>5.7</v>
@@ -5542,16 +5809,16 @@
       <c r="H3" s="79"/>
       <c r="I3" s="73"/>
       <c r="J3" s="89" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" s="68" customFormat="1" spans="1:10">
       <c r="A4" s="80"/>
       <c r="B4" s="81" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="C4" s="82" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="D4" s="83">
         <v>3.5</v>
@@ -5571,10 +5838,10 @@
     <row r="5" s="69" customFormat="1" spans="1:10">
       <c r="A5" s="80"/>
       <c r="B5" s="81" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C5" s="82" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="D5" s="83">
         <v>5.8</v>
@@ -5588,7 +5855,7 @@
       <c r="H5" s="79"/>
       <c r="I5" s="67"/>
       <c r="J5" s="89" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" s="68" customFormat="1" spans="1:10">
@@ -5596,10 +5863,10 @@
         <v>45957</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="C6" s="77" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D6" s="78">
         <v>23</v>
@@ -5624,10 +5891,10 @@
         <v>45958</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C7" s="82" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D7" s="83">
         <v>23</v>
@@ -5644,16 +5911,16 @@
       <c r="H7" s="79"/>
       <c r="I7" s="67"/>
       <c r="J7" s="89" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" s="68" customFormat="1" spans="1:10">
       <c r="A8" s="80"/>
       <c r="B8" s="81" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C8" s="82" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="D8" s="83">
         <v>5.3</v>
@@ -5675,10 +5942,10 @@
         <v>45959</v>
       </c>
       <c r="B9" s="76" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="C9" s="77" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="D9" s="78">
         <v>30</v>
@@ -5695,7 +5962,7 @@
       <c r="H9" s="79"/>
       <c r="I9" s="67"/>
       <c r="J9" s="89" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" s="68" customFormat="1" spans="1:10">
@@ -5703,10 +5970,10 @@
         <v>45960</v>
       </c>
       <c r="B10" s="81" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="C10" s="82" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="D10" s="83">
         <v>30</v>
@@ -5729,10 +5996,10 @@
     <row r="11" s="68" customFormat="1" spans="1:10">
       <c r="A11" s="80"/>
       <c r="B11" s="81" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="C11" s="82" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="D11" s="83">
         <v>11</v>
@@ -5746,16 +6013,16 @@
       <c r="H11" s="79"/>
       <c r="I11" s="67"/>
       <c r="J11" s="92" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" s="68" customFormat="1" spans="1:10">
       <c r="A12" s="80"/>
       <c r="B12" s="81" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C12" s="82" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D12" s="83">
         <v>12</v>
@@ -5776,10 +6043,10 @@
     <row r="13" s="68" customFormat="1" spans="1:10">
       <c r="A13" s="80"/>
       <c r="B13" s="81" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="C13" s="82" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D13" s="83">
         <v>11</v>
@@ -5793,16 +6060,16 @@
       <c r="H13" s="79"/>
       <c r="I13" s="67"/>
       <c r="J13" s="92" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" s="68" customFormat="1" spans="1:10">
       <c r="A14" s="80"/>
       <c r="B14" s="81" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="C14" s="82" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="D14" s="83">
         <v>12</v>
@@ -5823,10 +6090,10 @@
     <row r="15" s="68" customFormat="1" spans="1:10">
       <c r="A15" s="80"/>
       <c r="B15" s="81" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="C15" s="82" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="D15" s="83">
         <v>13.2</v>
@@ -5840,7 +6107,7 @@
       <c r="H15" s="79"/>
       <c r="I15" s="67"/>
       <c r="J15" s="92" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" s="68" customFormat="1" spans="1:10">
@@ -5848,10 +6115,10 @@
         <v>45961</v>
       </c>
       <c r="B16" s="76" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C16" s="77" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D16" s="78">
         <v>11.4</v>
@@ -5875,10 +6142,10 @@
     <row r="17" s="68" customFormat="1" spans="1:10">
       <c r="A17" s="75"/>
       <c r="B17" s="76" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="C17" s="77" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="D17" s="78">
         <v>12.6</v>
@@ -5892,7 +6159,7 @@
       <c r="H17" s="79"/>
       <c r="I17" s="67"/>
       <c r="J17" s="93" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" s="68" customFormat="1" spans="1:10">
@@ -5900,10 +6167,10 @@
         <v>45964</v>
       </c>
       <c r="B18" s="76" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C18" s="77" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D18" s="78">
         <v>24</v>
@@ -5927,10 +6194,10 @@
     <row r="19" s="68" customFormat="1" spans="1:9">
       <c r="A19" s="75"/>
       <c r="B19" s="76" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="C19" s="77" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="D19" s="78">
         <v>13.4</v>
@@ -5949,10 +6216,10 @@
         <v>45966</v>
       </c>
       <c r="B20" s="81" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C20" s="82" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="D20" s="83">
         <v>8.2</v>
@@ -5971,10 +6238,10 @@
     <row r="21" s="68" customFormat="1" spans="1:9">
       <c r="A21" s="80"/>
       <c r="B21" s="81" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="C21" s="82" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="D21" s="83">
         <v>27</v>
@@ -5991,10 +6258,10 @@
     <row r="22" spans="1:8">
       <c r="A22" s="80"/>
       <c r="B22" s="81" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="C22" s="82" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="D22" s="83">
         <v>22</v>
@@ -6012,10 +6279,10 @@
         <v>45967</v>
       </c>
       <c r="B23" s="77" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C23" s="77" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="D23" s="78">
         <v>24</v>
@@ -6034,10 +6301,10 @@
     <row r="24" spans="1:8">
       <c r="A24" s="75"/>
       <c r="B24" s="76" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="C24" s="77" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="D24" s="78">
         <v>12</v>
@@ -6055,10 +6322,10 @@
         <v>45969</v>
       </c>
       <c r="B25" s="81" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C25" s="82" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="D25" s="83">
         <v>12.4</v>
@@ -6079,10 +6346,10 @@
         <v>45971</v>
       </c>
       <c r="B26" s="76" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="C26" s="77" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="D26" s="78">
         <v>15.8</v>
@@ -6103,10 +6370,10 @@
         <v>45972</v>
       </c>
       <c r="B27" s="81" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C27" s="82" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D27" s="83">
         <v>13</v>
@@ -6127,10 +6394,10 @@
         <v>45974</v>
       </c>
       <c r="B28" s="76" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="C28" s="77" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="D28" s="78">
         <v>15</v>
@@ -6149,10 +6416,10 @@
     <row r="29" spans="1:8">
       <c r="A29" s="75"/>
       <c r="B29" s="76" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C29" s="77" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="D29" s="78">
         <v>20</v>
@@ -6217,31 +6484,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="H1" s="49" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="I1" s="49" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="J1" s="47" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" ht="129" customHeight="1" spans="1:13">
@@ -6249,16 +6516,16 @@
         <v>45967</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="D2" s="53">
         <v>3</v>
       </c>
       <c r="E2" s="54" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="F2" s="54" t="str">
         <f>_xlfn.DISPIMG("ID_A435215B813C404CA26F65668F85307D",1)</f>
@@ -6276,7 +6543,7 @@
         <v>846000</v>
       </c>
       <c r="J2" s="65" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="M2" s="66"/>
     </row>
@@ -6469,19 +6736,19 @@
   <sheetData>
     <row r="1" s="26" customFormat="1" ht="39.75" customHeight="1" spans="1:56">
       <c r="A1" s="27" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F1" s="29"/>
       <c r="G1" s="30"/>
@@ -6540,7 +6807,7 @@
         <v>45973</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="C2" s="31">
         <v>1000000</v>
@@ -6607,7 +6874,7 @@
         <v>45973</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="32">
@@ -6674,7 +6941,7 @@
         <v>45974</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="32">
@@ -6741,7 +7008,7 @@
         <v>45974</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="32">
@@ -6808,7 +7075,7 @@
         <v>45974</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="32">
@@ -6875,7 +7142,7 @@
         <v>45974</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="32">
@@ -6942,7 +7209,7 @@
         <v>45975</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="32">
@@ -7009,7 +7276,7 @@
         <v>45975</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="32">
@@ -11035,7 +11302,7 @@
       <c r="BB74" s="29"/>
       <c r="BC74" s="29"/>
       <c r="BD74" s="29" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
     </row>
     <row r="75" s="26" customFormat="1" ht="39.75" customHeight="1" spans="1:56">
@@ -13068,14 +13335,14 @@
   <sheetData>
     <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="7" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" ht="65" customHeight="1" spans="1:4">
@@ -13083,10 +13350,10 @@
         <v>45973</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D2" s="11" t="str">
         <f>_xlfn.DISPIMG("ID_FB2B4E78CDE640C7B889C532C0253C77",1)</f>
@@ -13098,10 +13365,10 @@
         <v>45973</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="D3" s="13"/>
     </row>
@@ -13110,10 +13377,10 @@
         <v>45974</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="D4" s="15" t="str">
         <f>_xlfn.DISPIMG("ID_1635F4017F2949E097AC01610113A384",1)</f>
@@ -13125,10 +13392,10 @@
         <v>45974</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D5" s="15" t="str">
         <f>_xlfn.DISPIMG("ID_B793726908DD4B3B9BADF1FE26DC0927",1)</f>
@@ -13140,10 +13407,10 @@
         <v>45974</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="D6" s="15" t="str">
         <f>_xlfn.DISPIMG("ID_78BBA2D7BAB14DEB93596E0834F3EC9F",1)</f>
@@ -13155,10 +13422,10 @@
         <v>45974</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="D7" s="15" t="str">
         <f>_xlfn.DISPIMG("ID_0A956BE1438E41B69C190696196303E1",1)</f>
@@ -13170,10 +13437,10 @@
         <v>45975</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="D8" s="21" t="str">
         <f>_xlfn.DISPIMG("ID_07F3A82E63C84F9385A92B06871CD739",1)</f>
@@ -13185,10 +13452,10 @@
         <v>45975</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D9" s="25" t="str">
         <f>_xlfn.DISPIMG("ID_94CE67D117E24BC4856DDEF6FF011A7B",1)</f>

</xml_diff>